<commit_message>
[23 June 2023] - maven project created by Sanjay sir but extent report and log4j added by me
</commit_message>
<xml_diff>
--- a/TestData/SeleniumRevisionC'wad.xlsx
+++ b/TestData/SeleniumRevisionC'wad.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83E00EC7-3997-40D7-A6AF-9E30E8FC8C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shree\git\SeleniumRevisionMaven1\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B278D8-6C2C-4C13-AB8C-BD05C0A1AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="2775" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="DDF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -391,12 +395,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -427,7 +431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
@@ -435,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100.5</v>
       </c>
@@ -443,7 +447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -464,9 +468,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,17 +484,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -504,13 +508,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668692A-5649-4473-B42D-EA9DE28AA914}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
[23 July 2023] Complete FrameWork
</commit_message>
<xml_diff>
--- a/TestData/SeleniumRevisionC'wad.xlsx
+++ b/TestData/SeleniumRevisionC'wad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shree\git\SeleniumRevisionMaven1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B278D8-6C2C-4C13-AB8C-BD05C0A1AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898C4C5F-9182-44E7-8FB9-D88A1A582D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="2775" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>abc</t>
   </si>
@@ -60,13 +60,19 @@
   </si>
   <si>
     <t>Jan batch</t>
+  </si>
+  <si>
+    <t>7020500587</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +87,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,10 +116,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,18 +520,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668692A-5649-4473-B42D-EA9DE28AA914}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="205" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>